<commit_message>
All WorksheetReader tests pass
</commit_message>
<xml_diff>
--- a/DataTransferer.Test/TestFiles/testFile.xlsx
+++ b/DataTransferer.Test/TestFiles/testFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr hidePivotFieldList="1"/>
   <bookViews>
-    <workbookView windowWidth="24041" windowHeight="9867" tabRatio="658"/>
+    <workbookView windowWidth="24041" windowHeight="9867" tabRatio="658" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Listopad2017" sheetId="1" r:id="rId1"/>
@@ -105,15 +105,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="dd/mm/yy\ h:mm;@"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00\ &quot;zł&quot;"/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="177" formatCode="dd/mm/yy\ h:mm;@"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="#,##0.00\ &quot;zł&quot;"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="yyyy/mm/dd;@"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +131,44 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -138,14 +176,90 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,127 +272,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -289,67 +282,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,25 +444,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,85 +462,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -480,15 +473,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -503,47 +487,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -567,6 +510,56 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -583,158 +576,158 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1056,8 +1049,8 @@
   <sheetPr/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1152,7 +1145,9 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <v>43261</v>
+      </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4">
@@ -1245,8 +1240,8 @@
   <sheetPr/>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
Added Currency enum, exceptions for SpendingsExcelDataParser, refactored ReadingSpreadsheetExceptions, started implementation of parsing spendings
</commit_message>
<xml_diff>
--- a/DataTransferer.Test/TestFiles/testFile.xlsx
+++ b/DataTransferer.Test/TestFiles/testFile.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>Data</t>
   </si>
@@ -107,13 +107,13 @@
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd;@"/>
     <numFmt numFmtId="177" formatCode="dd/mm/yy\ h:mm;@"/>
+    <numFmt numFmtId="178" formatCode="#,##0.00\ &quot;zł&quot;"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="#,##0.00\ &quot;zł&quot;"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +123,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -144,61 +151,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,65 +190,95 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -288,6 +295,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -300,12 +319,144 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -318,151 +469,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,6 +480,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -487,24 +503,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -524,26 +522,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -555,6 +533,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -573,127 +562,145 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -702,30 +709,31 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1155,7 +1163,7 @@
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="2"/>
@@ -1202,7 +1210,7 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="4">
+      <c r="A17" s="5">
         <v>40976.2604166667</v>
       </c>
       <c r="D17" s="2"/>
@@ -1212,7 +1220,7 @@
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="5">
+      <c r="A19" s="6">
         <v>36323.5739236111</v>
       </c>
       <c r="D19" s="2"/>
@@ -1238,13 +1246,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1295,17 +1303,13 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2">
-        <v>13.5</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>43076</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="2">
         <v>27.2</v>
       </c>
@@ -1331,9 +1335,7 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="2">
-        <v>4</v>
-      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
@@ -1358,12 +1360,7 @@
       <c r="A12" s="1">
         <v>43078</v>
       </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2">
-        <v>44.57</v>
-      </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
@@ -1372,9 +1369,7 @@
       <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13"/>
       <c r="D13" s="2">
         <v>5.99</v>
       </c>
@@ -1393,9 +1388,10 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15" s="1"/>
       <c r="D15" s="2"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1"/>

</xml_diff>